<commit_message>
general optimization of integration methods (elec, mech and US classic) using odeint.
</commit_message>
<xml_diff>
--- a/PointNICE/templates/log_MECH.xlsx
+++ b/PointNICE/templates/log_MECH.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Google Drive\PhD\NICE model\Output\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Theo\Documents\PointNICE\PointNICE\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8292"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8295"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -393,35 +393,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S1"/>
+  <dimension ref="A1:P1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N2" sqref="N2"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.62890625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.41796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.89453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.3671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.62890625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.41796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.62890625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.26171875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.41796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.89453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.47265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.26171875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.89453125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.05078125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -470,9 +473,6 @@
       <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>